<commit_message>
New Logo bmp, ppt, color palette
</commit_message>
<xml_diff>
--- a/ITProjectManagement/BA/SpecsWireframes/ThemeColorPalette001.xlsx
+++ b/ITProjectManagement/BA/SpecsWireframes/ThemeColorPalette001.xlsx
@@ -13,14 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="ThemeColors" sheetId="4" r:id="rId1"/>
-    <sheet name="BlueThemePalette" sheetId="1" r:id="rId2"/>
+    <sheet name="Aqua" sheetId="5" r:id="rId2"/>
+    <sheet name="BlueThemePalette" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="38">
   <si>
     <t>Color #</t>
   </si>
@@ -110,6 +111,30 @@
   </si>
   <si>
     <t>Version 0.1</t>
+  </si>
+  <si>
+    <t>3f</t>
+  </si>
+  <si>
+    <t>1f</t>
+  </si>
+  <si>
+    <t>5f</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>Highlights</t>
+  </si>
+  <si>
+    <t>Alerts &amp; Danger</t>
+  </si>
+  <si>
+    <t>Scheme</t>
+  </si>
+  <si>
+    <t>Normal</t>
   </si>
 </sst>
 </file>
@@ -181,7 +206,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,8 +285,80 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3F9FFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00BFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3FFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7FFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7F00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDFFF1F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF7F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0F5FBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -493,11 +590,366 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -573,6 +1025,117 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,16 +1144,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFFF7F4F"/>
-      <color rgb="FF4F7FFF"/>
-      <color rgb="FF6F6FFF"/>
-      <color rgb="FF5F5FFF"/>
-      <color rgb="FF19C139"/>
-      <color rgb="FFFF9900"/>
-      <color rgb="FF7F0F0F"/>
-      <color rgb="FFAF4F4F"/>
-      <color rgb="FFFFEFEF"/>
-      <color rgb="FFFFDFDF"/>
+      <color rgb="FF3FFFFF"/>
+      <color rgb="FF3F9FFF"/>
+      <color rgb="FF0F5FBF"/>
+      <color rgb="FF0F5F9F"/>
+      <color rgb="FF0F9F5F"/>
+      <color rgb="FF00BFBF"/>
+      <color rgb="FF0F9F7F"/>
+      <color rgb="FF1F7FBF"/>
+      <color rgb="FF0F5F7F"/>
+      <color rgb="FF005FBF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -999,26 +1562,392 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="7.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="72">
+        <v>1</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="59">
+        <v>15</v>
+      </c>
+      <c r="E3" s="59">
+        <v>95</v>
+      </c>
+      <c r="F3" s="59">
+        <v>191</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="66" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="67"/>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="73">
+        <v>2</v>
+      </c>
+      <c r="C4" s="57"/>
+      <c r="D4" s="2">
+        <v>63</v>
+      </c>
+      <c r="E4" s="2">
+        <v>159</v>
+      </c>
+      <c r="F4" s="2">
+        <v>255</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="65"/>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="73">
+        <v>3</v>
+      </c>
+      <c r="C5" s="57"/>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>191</v>
+      </c>
+      <c r="F5" s="2">
+        <v>255</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="44"/>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="73">
+        <v>4</v>
+      </c>
+      <c r="C6" s="57"/>
+      <c r="D6" s="2">
+        <v>63</v>
+      </c>
+      <c r="E6" s="2">
+        <v>255</v>
+      </c>
+      <c r="F6" s="2">
+        <v>255</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="45"/>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="74">
+        <v>5</v>
+      </c>
+      <c r="C7" s="57"/>
+      <c r="D7" s="2">
+        <v>191</v>
+      </c>
+      <c r="E7" s="2">
+        <v>255</v>
+      </c>
+      <c r="F7" s="2">
+        <v>255</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="46"/>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="75">
+        <v>6</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="2">
+        <v>255</v>
+      </c>
+      <c r="E8" s="2">
+        <v>255</v>
+      </c>
+      <c r="F8" s="2">
+        <v>255</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="47"/>
+    </row>
+    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="76">
+        <v>7</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="63">
+        <v>255</v>
+      </c>
+      <c r="E9" s="63">
+        <v>127</v>
+      </c>
+      <c r="F9" s="63">
+        <v>0</v>
+      </c>
+      <c r="G9" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="63" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="48"/>
+    </row>
+    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="73">
+        <v>8</v>
+      </c>
+      <c r="C10" s="40"/>
+      <c r="D10" s="2">
+        <v>255</v>
+      </c>
+      <c r="E10" s="2">
+        <v>191</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="49"/>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="77">
+        <v>9</v>
+      </c>
+      <c r="C11" s="56"/>
+      <c r="D11" s="42">
+        <v>223</v>
+      </c>
+      <c r="E11" s="42">
+        <v>255</v>
+      </c>
+      <c r="F11" s="42">
+        <v>31</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="50"/>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="78">
+        <v>10</v>
+      </c>
+      <c r="C12" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="59">
+        <v>0</v>
+      </c>
+      <c r="E12" s="59">
+        <v>255</v>
+      </c>
+      <c r="F12" s="59">
+        <v>127</v>
+      </c>
+      <c r="G12" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="51"/>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="73">
+        <v>11</v>
+      </c>
+      <c r="C13" s="40"/>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>255</v>
+      </c>
+      <c r="F13" s="2">
+        <v>191</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="52"/>
+    </row>
+    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="79">
+        <v>12</v>
+      </c>
+      <c r="C14" s="56"/>
+      <c r="D14" s="42">
+        <v>255</v>
+      </c>
+      <c r="E14" s="42">
+        <v>127</v>
+      </c>
+      <c r="F14" s="42">
+        <v>255</v>
+      </c>
+      <c r="G14" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="53"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C3:C8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="H7:I14 I5 G5 G9:G14 I6" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="8" width="6.7109375" customWidth="1"/>
     <col min="9" max="9" width="32.5703125" customWidth="1"/>
+    <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1974,7 @@
       </c>
       <c r="J2" s="26"/>
     </row>
-    <row r="3" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="27">
         <v>1</v>
       </c>
@@ -1070,7 +1999,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="28"/>
     </row>
-    <row r="4" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="27">
         <v>2</v>
       </c>
@@ -1095,7 +2024,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="28"/>
     </row>
-    <row r="5" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="27">
         <v>3</v>
       </c>
@@ -1120,7 +2049,7 @@
       <c r="I5" s="13"/>
       <c r="J5" s="28"/>
     </row>
-    <row r="6" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="27">
         <v>4</v>
       </c>
@@ -1145,7 +2074,7 @@
       <c r="I6" s="14"/>
       <c r="J6" s="28"/>
     </row>
-    <row r="7" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="27">
         <v>5</v>
       </c>
@@ -1170,7 +2099,7 @@
       <c r="I7" s="15"/>
       <c r="J7" s="28"/>
     </row>
-    <row r="8" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="27">
         <v>6</v>
       </c>
@@ -1195,7 +2124,7 @@
       <c r="I8" s="16"/>
       <c r="J8" s="28"/>
     </row>
-    <row r="9" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="27">
         <v>7</v>
       </c>
@@ -1220,7 +2149,7 @@
       <c r="I9" s="17"/>
       <c r="J9" s="28"/>
     </row>
-    <row r="10" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="27">
         <v>8</v>
       </c>
@@ -1245,7 +2174,7 @@
       <c r="I10" s="18"/>
       <c r="J10" s="28"/>
     </row>
-    <row r="11" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="27">
         <v>9</v>
       </c>
@@ -1270,7 +2199,7 @@
       <c r="I11" s="19"/>
       <c r="J11" s="28"/>
     </row>
-    <row r="12" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="27">
         <v>10</v>
       </c>
@@ -1295,7 +2224,7 @@
       <c r="I12" s="20"/>
       <c r="J12" s="28"/>
     </row>
-    <row r="13" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="27">
         <v>11</v>
       </c>
@@ -1320,7 +2249,7 @@
       <c r="I13" s="21"/>
       <c r="J13" s="28"/>
     </row>
-    <row r="14" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="27">
         <v>12</v>
       </c>
@@ -1345,7 +2274,7 @@
       <c r="I14" s="22"/>
       <c r="J14" s="28"/>
     </row>
-    <row r="15" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="29">
         <v>13</v>
       </c>

</xml_diff>